<commit_message>
se agrega notebook de creacion de nuevas variables
</commit_message>
<xml_diff>
--- a/data/in/diccionario_datos.xlsx
+++ b/data/in/diccionario_datos.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22733767-B7B1-4A0B-83EC-C5D66C133674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F38213-8E7F-4393-A8DE-F64F891A1B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +303,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -361,10 +373,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -650,11 +671,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" style="4" customWidth="1"/>
@@ -810,30 +831,30 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -853,86 +874,86 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="B16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="B20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="14" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>